<commit_message>
done done. figures ready. report otw
</commit_message>
<xml_diff>
--- a/dataFigures.xlsx
+++ b/dataFigures.xlsx
@@ -35,7 +35,7 @@
     <t>mySpinTTAS time(ms)</t>
   </si>
   <si>
-    <t>myMutexTAS time(ms)</t>
+    <t>myMutexTTAS time(ms)</t>
   </si>
   <si>
     <t>myQueueLock time(ms)</t>
@@ -66,11 +66,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -86,6 +87,23 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="13"/>
@@ -145,7 +163,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -221,7 +239,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -235,7 +253,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300">
+              <a:rPr b="1" sz="1300">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Time(ms) Vary in Number of Threads</a:t>
@@ -276,7 +294,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -321,31 +339,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>137</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>511</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>887</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1041</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1300</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1608</c:v>
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>496</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>941</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1121</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1268</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1722</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1664</c:v>
+                  <c:v>1969</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1881</c:v>
+                  <c:v>2019</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -377,7 +395,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -425,28 +443,28 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>167</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>284</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>510</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>580</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>555</c:v>
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>285</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>321</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>722</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>670</c:v>
+                  <c:v>894</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>778</c:v>
+                  <c:v>1088</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -478,7 +496,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -523,31 +541,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>172</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>192</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>410</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>603</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>777</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>993</c:v>
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>269</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>426</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>710</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1105</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1458</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1863</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1182</c:v>
+                  <c:v>2130</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1514</c:v>
+                  <c:v>2757</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -579,7 +597,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -624,31 +642,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>143</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>229</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>266</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>382</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>572</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>898</c:v>
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>339</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>609</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>820</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>822</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1171</c:v>
+                  <c:v>1116</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1435</c:v>
+                  <c:v>1045</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -663,7 +681,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>myMutexTAS time(ms)</c:v>
+                  <c:v>myMutexTTAS time(ms)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -680,7 +698,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -725,31 +743,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>71</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>105</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>141</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>173</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>318</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>260</c:v>
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>358</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>409</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>387</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>337</c:v>
+                  <c:v>433</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>511</c:v>
+                  <c:v>723</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -781,7 +799,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -826,41 +844,41 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>152</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>267</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>347</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>442</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>586</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>663</c:v>
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>372</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>527</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>671</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>817</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>965</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>769</c:v>
+                  <c:v>1251</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4000</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="81276834"/>
-        <c:axId val="67259268"/>
+        <c:axId val="4696285"/>
+        <c:axId val="51205953"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81276834"/>
+        <c:axId val="4696285"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -876,7 +894,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Thread</a:t>
@@ -896,14 +914,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="67259268"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="51205953"/>
+        <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67259268"/>
+        <c:axId val="51205953"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="2000"/>
+          <c:max val="3000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -926,7 +944,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Time(ms)</a:t>
@@ -946,8 +964,8 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="81276834"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="4696285"/>
+        <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -979,7 +997,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -996,7 +1014,7 @@
               <a:rPr sz="1300">
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>Time(ms) Vary in Number of Iterations</a:t>
+              <a:t>Time(ms) Vary in Number of workOutsideCS</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1013,7 +1031,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$32:$B$32</c:f>
+              <c:f>Sheet1!$B$62</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1034,82 +1052,70 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$33:$A$42</c:f>
+              <c:f>Sheet1!$A$63:$A$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2000000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3000000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4000000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5000000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6000000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7000000</c:v>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9000000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10000000</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$33:$B$42</c:f>
+              <c:f>Sheet1!$B$63:$B$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>772</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1012.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2877</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3896</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4576</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5686</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6614</c:v>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>989</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>918</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1086</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1111</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>936</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>963</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7779</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8914</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9269</c:v>
+                  <c:v>845</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1120,7 +1126,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$32:$C$32</c:f>
+              <c:f>Sheet1!$C$62</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1141,82 +1147,70 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$33:$A$42</c:f>
+              <c:f>Sheet1!$A$63:$A$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2000000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3000000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4000000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5000000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6000000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7000000</c:v>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9000000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10000000</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$33:$C$42</c:f>
+              <c:f>Sheet1!$C$63:$C$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>391</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>577</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1121</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1038</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1899</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1544</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1840</c:v>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>277</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>442</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>502</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>353</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3007</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3426</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3773</c:v>
+                  <c:v>406</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1227,7 +1221,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$32:$D$32</c:f>
+              <c:f>Sheet1!$D$62</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1248,82 +1242,70 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$33:$A$42</c:f>
+              <c:f>Sheet1!$A$63:$A$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2000000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3000000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4000000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5000000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6000000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7000000</c:v>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9000000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10000000</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$33:$D$42</c:f>
+              <c:f>Sheet1!$D$63:$D$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>379</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>863</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1251</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1312</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1857</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2371</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2818</c:v>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>839</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>764</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>790</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>755</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>671</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>681</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>634</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2490</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3576</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3941</c:v>
+                  <c:v>596</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1334,7 +1316,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$32:$E$32</c:f>
+              <c:f>Sheet1!$E$62</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1355,82 +1337,70 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$33:$A$42</c:f>
+              <c:f>Sheet1!$A$63:$A$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2000000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3000000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4000000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5000000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6000000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7000000</c:v>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9000000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10000000</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$33:$E$42</c:f>
+              <c:f>Sheet1!$E$63:$E$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>263</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>668</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>917</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1468</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1571</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1856</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1930</c:v>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>487</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>501</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>565</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>643</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>634</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>559</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2141</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2468</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2685</c:v>
+                  <c:v>551</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1441,11 +1411,11 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$32:$F$32</c:f>
+              <c:f>Sheet1!$F$62</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>myMutexTAS time(ms)</c:v>
+                  <c:v>myMutexTTAS time(ms)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1462,82 +1432,70 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$33:$A$42</c:f>
+              <c:f>Sheet1!$A$63:$A$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2000000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3000000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4000000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5000000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6000000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7000000</c:v>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9000000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10000000</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$33:$F$42</c:f>
+              <c:f>Sheet1!$F$63:$F$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>129</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>404</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>567</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>769</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>969</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1035</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1510</c:v>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>398</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>544</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>539</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>559</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>865</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1507</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2023</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2552</c:v>
+                  <c:v>901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1548,7 +1506,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$32:$G$32</c:f>
+              <c:f>Sheet1!$G$62</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1569,92 +1527,80 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$33:$A$42</c:f>
+              <c:f>Sheet1!$A$63:$A$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2000000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3000000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4000000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5000000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6000000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7000000</c:v>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9000000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10000000</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$33:$G$42</c:f>
+              <c:f>Sheet1!$G$63:$G$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>365</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>729</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1050</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1383</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1755</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2188</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2465</c:v>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>536</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>546</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>524</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>514</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>519</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>529</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>510</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2847</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3134</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3502</c:v>
+                  <c:v>531</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="44371107"/>
-        <c:axId val="25467475"/>
+        <c:axId val="71128404"/>
+        <c:axId val="29269846"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44371107"/>
+        <c:axId val="71128404"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1673,7 +1619,7 @@
                   <a:rPr sz="900">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>Iteration</a:t>
+                  <a:t>workOutsideCS</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1690,11 +1636,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="25467475"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="29269846"/>
+        <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="25467475"/>
+        <c:axId val="29269846"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1739,7 +1685,840 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="44371107"/>
+        <c:crossAx val="71128404"/>
+        <c:crossesAt val="0"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1300">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Time(ms) Vary in Number of Iterations</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pthread Mutex time(ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$33:$A$42</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$33:$B$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>17451</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1822</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>779</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>664</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>796</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>990</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>935</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>963</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pthread Spinlock time(ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$33:$A$42</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$33:$C$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9394</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>879</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>279</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>309</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>281</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>286</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>285</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>mySpinTAS time(ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$33:$A$42</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$33:$D$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10276</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>769</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>805</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>407</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>752</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>727</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>856</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>mySpinTTAS time(ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="579d1c"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$33:$A$42</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$33:$E$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5610</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1138</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>368</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>402</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>363</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>366</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>423</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>454</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>470</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>myMutexTTAS time(ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="7e0021"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$33:$A$42</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$33:$F$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>6660</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1499</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>284</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>390</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>myQueueLock time(ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="83caff"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="7"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$33:$A$42</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4000000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5000000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$33:$G$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>8960</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>398</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>573</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>579</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>515</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>515</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>519</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>540</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="6693344"/>
+        <c:axId val="614262"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="6693344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Iteration</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="614262"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="614262"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="9000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Time(ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="6693344"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1772,10 +2551,30 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1300">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Time(ms) Vary in Number of workInsideCS</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -1786,7 +2585,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$62</c:f>
+              <c:f>Sheet1!$B$92</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1811,84 +2610,60 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$63:$A$73</c:f>
+              <c:f>Sheet1!$A$93:$A$99</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="1">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$63:$B$73</c:f>
+              <c:f>Sheet1!$B$93:$B$99</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>886</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>925</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>725</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>824</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>892</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>898</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>774</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1006</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>908</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>979</c:v>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>970</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1566</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2139</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2255</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2313</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2184</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1899,7 +2674,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$62</c:f>
+              <c:f>Sheet1!$C$92</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1924,84 +2699,60 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$63:$A$73</c:f>
+              <c:f>Sheet1!$A$93:$A$99</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="1">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$63:$C$73</c:f>
+              <c:f>Sheet1!$C$93:$C$99</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>233</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>314</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>311</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>337</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>294</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>294</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>279</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>343</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>266</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>208</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>340</c:v>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>474</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>615</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>773</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1013</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>934</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1497</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2012,7 +2763,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$62</c:f>
+              <c:f>Sheet1!$D$92</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2037,84 +2788,60 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$63:$A$73</c:f>
+              <c:f>Sheet1!$A$93:$A$99</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="1">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$63:$D$73</c:f>
+              <c:f>Sheet1!$D$93:$D$99</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>436</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>376</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>406</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>532</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>488</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>459</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>413</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>599</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>583</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>493</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>452</c:v>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>789</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1032</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1171</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1444</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1395</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1486</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2125,7 +2852,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$62</c:f>
+              <c:f>Sheet1!$E$92</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2150,84 +2877,60 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$63:$A$73</c:f>
+              <c:f>Sheet1!$A$93:$A$99</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="1">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$63:$E$73</c:f>
+              <c:f>Sheet1!$E$93:$E$99</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>352</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>356</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>320</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>435</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>358</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>379</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>418</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>407</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>421</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>404</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>408</c:v>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>401</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>437</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>568</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>709</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>814</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>857</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2238,11 +2941,11 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$62</c:f>
+              <c:f>Sheet1!$F$92</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>myMutexTAS time(ms)</c:v>
+                  <c:v>myMutexTTAS time(ms)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2263,84 +2966,60 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$63:$A$73</c:f>
+              <c:f>Sheet1!$A$93:$A$99</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="1">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$63:$F$73</c:f>
+              <c:f>Sheet1!$F$93:$F$99</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>238</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>137</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>167</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>148</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>241</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>162</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>169</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>257</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>348</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>255</c:v>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>339</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>554</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>548</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>637</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2351,7 +3030,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$62</c:f>
+              <c:f>Sheet1!$G$92</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2376,99 +3055,95 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$63:$A$73</c:f>
+              <c:f>Sheet1!$A$93:$A$99</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="1">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$63:$G$73</c:f>
+              <c:f>Sheet1!$G$93:$G$99</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>345</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>346</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>370</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>361</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>374</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>324</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>357</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>353</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>339</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>350</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>362</c:v>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>515</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>595</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>696</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>862</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>865</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>992</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="80929511"/>
-        <c:axId val="88008875"/>
+        <c:axId val="99921654"/>
+        <c:axId val="63278491"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80929511"/>
+        <c:axId val="99921654"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>workInsideCS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2479,11 +3154,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="88008875"/>
+        <c:crossAx val="63278491"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88008875"/>
+        <c:axId val="63278491"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2498,6 +3173,26 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Time(ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2508,7 +3203,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="80929511"/>
+        <c:crossAx val="99921654"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2521,8 +3216,6 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2548,15 +3241,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>803520</xdr:colOff>
+      <xdr:colOff>10440</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>11160</xdr:rowOff>
+      <xdr:rowOff>27360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>468000</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>68400</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>806760</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>135360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2564,8 +3257,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="13252680" y="173520"/>
-        <a:ext cx="6166800" cy="3796200"/>
+        <a:off x="12459600" y="189720"/>
+        <a:ext cx="6485760" cy="4659840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2577,16 +3270,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>811440</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>40680</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1618560</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>153360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>506160</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>149040</xdr:rowOff>
+      <xdr:colOff>9720</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>162720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2594,8 +3287,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="13260600" y="4754880"/>
-        <a:ext cx="6197040" cy="4172400"/>
+        <a:off x="12440520" y="9906840"/>
+        <a:ext cx="6520680" cy="4723560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2608,15 +3301,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>36360</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
+      <xdr:colOff>36720</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>149040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>106560</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>24120</xdr:rowOff>
+      <xdr:colOff>741240</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2624,12 +3317,42 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="12485520" y="9951840"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="12485880" y="5025600"/>
+        <a:ext cx="6393960" cy="4646520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1598040</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>22680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>780480</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>122040</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="12420000" y="14815440"/>
+        <a:ext cx="6499080" cy="4813560"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2643,10 +3366,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G102"/>
+  <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F81" activeCellId="0" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2698,22 +3421,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>10</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2721,22 +3444,22 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>100</v>
+        <v>29</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>172</v>
+        <v>269</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>152</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2744,22 +3467,22 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>511</v>
+        <v>496</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>192</v>
+        <v>426</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>229</v>
+        <v>251</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>105</v>
+        <v>137</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>267</v>
+        <v>372</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2767,22 +3490,22 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>887</v>
+        <v>941</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>410</v>
+        <v>710</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>266</v>
+        <v>339</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>141</v>
+        <v>200</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>347</v>
+        <v>527</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2790,22 +3513,22 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>1041</v>
+        <v>1121</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>510</v>
+        <v>321</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>603</v>
+        <v>1105</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>382</v>
+        <v>609</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>173</v>
+        <v>358</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>442</v>
+        <v>671</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2813,22 +3536,22 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>1300</v>
+        <v>1268</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>580</v>
+        <v>320</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>777</v>
+        <v>1458</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>572</v>
+        <v>820</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>318</v>
+        <v>409</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>586</v>
+        <v>817</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2836,22 +3559,22 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>1608</v>
+        <v>1722</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>555</v>
+        <v>722</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>993</v>
+        <v>1863</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>898</v>
+        <v>822</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>260</v>
+        <v>387</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>663</v>
+        <v>965</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2859,22 +3582,22 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>1664</v>
+        <v>1969</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>670</v>
+        <v>894</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>1182</v>
+        <v>2130</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>1171</v>
+        <v>1116</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>337</v>
+        <v>433</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>769</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2882,22 +3605,22 @@
         <v>9</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>1881</v>
+        <v>2019</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>778</v>
+        <v>1088</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>1514</v>
+        <v>2757</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>1435</v>
+        <v>1045</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>511</v>
+        <v>723</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>4000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2935,233 +3658,232 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>1000000</v>
+        <v>10</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>772</v>
+        <v>17451</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>391</v>
+        <v>9394</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>379</v>
+        <v>10276</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>263</v>
+        <v>5610</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>129</v>
+        <v>6660</v>
       </c>
       <c r="G33" s="0" t="n">
-        <v>365</v>
+        <v>8960</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>2000000</v>
+        <v>100</v>
       </c>
       <c r="B34" s="0" t="n">
-        <f aca="false">(2025*A33)/A34</f>
-        <v>1012.5</v>
+        <v>1822</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>577</v>
+        <v>879</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>863</v>
+        <v>769</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>668</v>
+        <v>1138</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>404</v>
+        <v>1499</v>
       </c>
       <c r="G34" s="0" t="n">
-        <v>729</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>3000000</v>
+        <v>1000</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>2877</v>
+        <v>154</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>1121</v>
+        <v>97</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>1251</v>
+        <v>143</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>917</v>
+        <v>181</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>567</v>
+        <v>221</v>
       </c>
       <c r="G35" s="0" t="n">
-        <v>1050</v>
+        <v>398</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
-        <v>4000000</v>
+        <v>10000</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>3896</v>
+        <v>779</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>1038</v>
+        <v>279</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>1312</v>
+        <v>805</v>
       </c>
       <c r="E36" s="0" t="n">
-        <v>1468</v>
+        <v>368</v>
       </c>
       <c r="F36" s="0" t="n">
-        <v>769</v>
+        <v>165</v>
       </c>
       <c r="G36" s="0" t="n">
-        <v>1383</v>
+        <v>573</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>5000000</v>
+        <v>100000</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>4576</v>
+        <v>664</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>1899</v>
+        <v>92</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>1857</v>
+        <v>407</v>
       </c>
       <c r="E37" s="0" t="n">
-        <v>1571</v>
+        <v>402</v>
       </c>
       <c r="F37" s="0" t="n">
-        <v>969</v>
+        <v>161</v>
       </c>
       <c r="G37" s="0" t="n">
-        <v>1755</v>
+        <v>579</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>6000000</v>
+        <v>1000000</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>5686</v>
+        <v>796</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>1544</v>
+        <v>290</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>2371</v>
+        <v>752</v>
       </c>
       <c r="E38" s="0" t="n">
-        <v>1856</v>
+        <v>363</v>
       </c>
       <c r="F38" s="0" t="n">
-        <v>1035</v>
+        <v>320</v>
       </c>
       <c r="G38" s="0" t="n">
-        <v>2188</v>
+        <v>515</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>7000000</v>
+        <v>2000000</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>6614</v>
+        <v>990</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>1840</v>
+        <v>309</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>2818</v>
+        <v>720</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>1930</v>
+        <v>366</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>1510</v>
+        <v>208</v>
       </c>
       <c r="G39" s="0" t="n">
-        <v>2465</v>
+        <v>520</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
-        <v>8000000</v>
+        <v>3000000</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>7779</v>
+        <v>950</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>3007</v>
+        <v>281</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>2490</v>
+        <v>727</v>
       </c>
       <c r="E40" s="0" t="n">
-        <v>2141</v>
+        <v>423</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>1507</v>
+        <v>284</v>
       </c>
       <c r="G40" s="0" t="n">
-        <v>2847</v>
+        <v>515</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
-        <v>9000000</v>
+        <v>4000000</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>8914</v>
+        <v>935</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>3426</v>
+        <v>286</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>3576</v>
+        <v>856</v>
       </c>
       <c r="E41" s="0" t="n">
-        <v>2468</v>
+        <v>454</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>2023</v>
+        <v>256</v>
       </c>
       <c r="G41" s="0" t="n">
-        <v>3134</v>
+        <v>519</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
-        <v>10000000</v>
+        <v>5000000</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>9269</v>
+        <v>963</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>3773</v>
+        <v>285</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>3941</v>
+        <v>700</v>
       </c>
       <c r="E42" s="0" t="n">
-        <v>2685</v>
+        <v>470</v>
       </c>
       <c r="F42" s="0" t="n">
-        <v>2552</v>
+        <v>390</v>
       </c>
       <c r="G42" s="0" t="n">
-        <v>3502</v>
+        <v>540</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3202,22 +3924,22 @@
         <v>0</v>
       </c>
       <c r="B63" s="0" t="n">
-        <v>886</v>
+        <v>989</v>
       </c>
       <c r="C63" s="0" t="n">
-        <v>233</v>
+        <v>193</v>
       </c>
       <c r="D63" s="0" t="n">
-        <v>436</v>
+        <v>839</v>
       </c>
       <c r="E63" s="0" t="n">
-        <v>352</v>
+        <v>487</v>
       </c>
       <c r="F63" s="0" t="n">
-        <v>128</v>
+        <v>213</v>
       </c>
       <c r="G63" s="0" t="n">
-        <v>345</v>
+        <v>536</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3225,229 +3947,160 @@
         <v>1</v>
       </c>
       <c r="B64" s="0" t="n">
-        <v>925</v>
+        <v>918</v>
       </c>
       <c r="C64" s="0" t="n">
-        <v>314</v>
+        <v>277</v>
       </c>
       <c r="D64" s="0" t="n">
-        <v>376</v>
+        <v>764</v>
       </c>
       <c r="E64" s="0" t="n">
-        <v>356</v>
+        <v>501</v>
       </c>
       <c r="F64" s="0" t="n">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="G64" s="0" t="n">
-        <v>346</v>
+        <v>546</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B65" s="0" t="n">
-        <v>725</v>
+        <v>1086</v>
       </c>
       <c r="C65" s="0" t="n">
-        <v>311</v>
+        <v>442</v>
       </c>
       <c r="D65" s="0" t="n">
-        <v>406</v>
+        <v>790</v>
       </c>
       <c r="E65" s="0" t="n">
-        <v>320</v>
+        <v>565</v>
       </c>
       <c r="F65" s="0" t="n">
-        <v>137</v>
+        <v>398</v>
       </c>
       <c r="G65" s="0" t="n">
-        <v>370</v>
+        <v>524</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B66" s="0" t="n">
-        <v>824</v>
+        <v>1111</v>
       </c>
       <c r="C66" s="0" t="n">
-        <v>337</v>
+        <v>315</v>
       </c>
       <c r="D66" s="0" t="n">
-        <v>532</v>
+        <v>755</v>
       </c>
       <c r="E66" s="0" t="n">
-        <v>435</v>
+        <v>643</v>
       </c>
       <c r="F66" s="0" t="n">
-        <v>167</v>
+        <v>544</v>
       </c>
       <c r="G66" s="0" t="n">
-        <v>361</v>
+        <v>514</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B67" s="0" t="n">
-        <v>892</v>
+        <v>1014</v>
       </c>
       <c r="C67" s="0" t="n">
-        <v>294</v>
+        <v>502</v>
       </c>
       <c r="D67" s="0" t="n">
-        <v>488</v>
+        <v>671</v>
       </c>
       <c r="E67" s="0" t="n">
-        <v>358</v>
+        <v>634</v>
       </c>
       <c r="F67" s="0" t="n">
-        <v>148</v>
+        <v>539</v>
       </c>
       <c r="G67" s="0" t="n">
-        <v>374</v>
+        <v>519</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="B68" s="0" t="n">
-        <v>898</v>
+        <v>936</v>
       </c>
       <c r="C68" s="0" t="n">
-        <v>294</v>
+        <v>355</v>
       </c>
       <c r="D68" s="0" t="n">
-        <v>459</v>
+        <v>681</v>
       </c>
       <c r="E68" s="0" t="n">
-        <v>379</v>
+        <v>590</v>
       </c>
       <c r="F68" s="0" t="n">
-        <v>241</v>
+        <v>559</v>
       </c>
       <c r="G68" s="0" t="n">
-        <v>324</v>
+        <v>529</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B69" s="0" t="n">
-        <v>1024</v>
+        <v>963</v>
       </c>
       <c r="C69" s="0" t="n">
-        <v>279</v>
+        <v>353</v>
       </c>
       <c r="D69" s="0" t="n">
-        <v>413</v>
+        <v>634</v>
       </c>
       <c r="E69" s="0" t="n">
-        <v>418</v>
+        <v>559</v>
       </c>
       <c r="F69" s="0" t="n">
-        <v>162</v>
+        <v>865</v>
       </c>
       <c r="G69" s="0" t="n">
-        <v>357</v>
+        <v>510</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="B70" s="0" t="n">
-        <v>774</v>
+        <v>845</v>
       </c>
       <c r="C70" s="0" t="n">
-        <v>343</v>
+        <v>406</v>
       </c>
       <c r="D70" s="0" t="n">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="E70" s="0" t="n">
-        <v>407</v>
+        <v>551</v>
       </c>
       <c r="F70" s="0" t="n">
-        <v>169</v>
+        <v>901</v>
       </c>
       <c r="G70" s="0" t="n">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B71" s="0" t="n">
-        <v>1006</v>
-      </c>
-      <c r="C71" s="0" t="n">
-        <v>266</v>
-      </c>
-      <c r="D71" s="0" t="n">
-        <v>583</v>
-      </c>
-      <c r="E71" s="0" t="n">
-        <v>421</v>
-      </c>
-      <c r="F71" s="0" t="n">
-        <v>257</v>
-      </c>
-      <c r="G71" s="0" t="n">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="B72" s="0" t="n">
-        <v>908</v>
-      </c>
-      <c r="C72" s="0" t="n">
-        <v>208</v>
-      </c>
-      <c r="D72" s="0" t="n">
-        <v>493</v>
-      </c>
-      <c r="E72" s="0" t="n">
-        <v>404</v>
-      </c>
-      <c r="F72" s="0" t="n">
-        <v>348</v>
-      </c>
-      <c r="G72" s="0" t="n">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B73" s="0" t="n">
-        <v>979</v>
-      </c>
-      <c r="C73" s="0" t="n">
-        <v>340</v>
-      </c>
-      <c r="D73" s="0" t="n">
-        <v>452</v>
-      </c>
-      <c r="E73" s="0" t="n">
-        <v>408</v>
-      </c>
-      <c r="F73" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="G73" s="0" t="n">
-        <v>362</v>
+        <v>531</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3487,50 +4140,161 @@
       <c r="A93" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="B93" s="0" t="n">
+        <v>970</v>
+      </c>
+      <c r="C93" s="0" t="n">
+        <v>270</v>
+      </c>
+      <c r="D93" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="E93" s="0" t="n">
+        <v>401</v>
+      </c>
+      <c r="F93" s="0" t="n">
+        <v>187</v>
+      </c>
+      <c r="G93" s="0" t="n">
+        <v>515</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="n">
-        <v>2</v>
+        <v>10</v>
+      </c>
+      <c r="B94" s="0" t="n">
+        <v>1265</v>
+      </c>
+      <c r="C94" s="0" t="n">
+        <v>474</v>
+      </c>
+      <c r="D94" s="0" t="n">
+        <v>789</v>
+      </c>
+      <c r="E94" s="0" t="n">
+        <v>437</v>
+      </c>
+      <c r="F94" s="0" t="n">
+        <v>210</v>
+      </c>
+      <c r="G94" s="0" t="n">
+        <v>595</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="n">
-        <v>3</v>
+        <v>20</v>
+      </c>
+      <c r="B95" s="0" t="n">
+        <v>1566</v>
+      </c>
+      <c r="C95" s="0" t="n">
+        <v>615</v>
+      </c>
+      <c r="D95" s="0" t="n">
+        <v>1032</v>
+      </c>
+      <c r="E95" s="0" t="n">
+        <v>568</v>
+      </c>
+      <c r="F95" s="0" t="n">
+        <v>339</v>
+      </c>
+      <c r="G95" s="0" t="n">
+        <v>700</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="n">
-        <v>4</v>
+        <v>30</v>
+      </c>
+      <c r="B96" s="0" t="n">
+        <v>2139</v>
+      </c>
+      <c r="C96" s="0" t="n">
+        <v>773</v>
+      </c>
+      <c r="D96" s="0" t="n">
+        <v>1171</v>
+      </c>
+      <c r="E96" s="0" t="n">
+        <v>620</v>
+      </c>
+      <c r="F96" s="0" t="n">
+        <v>554</v>
+      </c>
+      <c r="G96" s="0" t="n">
+        <v>696</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="n">
-        <v>5</v>
+        <v>40</v>
+      </c>
+      <c r="B97" s="0" t="n">
+        <v>2255</v>
+      </c>
+      <c r="C97" s="0" t="n">
+        <v>1013</v>
+      </c>
+      <c r="D97" s="0" t="n">
+        <v>1444</v>
+      </c>
+      <c r="E97" s="0" t="n">
+        <v>709</v>
+      </c>
+      <c r="F97" s="0" t="n">
+        <v>548</v>
+      </c>
+      <c r="G97" s="0" t="n">
+        <v>862</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="n">
-        <v>6</v>
+        <v>50</v>
+      </c>
+      <c r="B98" s="0" t="n">
+        <v>2313</v>
+      </c>
+      <c r="C98" s="0" t="n">
+        <v>934</v>
+      </c>
+      <c r="D98" s="0" t="n">
+        <v>1395</v>
+      </c>
+      <c r="E98" s="0" t="n">
+        <v>814</v>
+      </c>
+      <c r="F98" s="0" t="n">
+        <v>860</v>
+      </c>
+      <c r="G98" s="0" t="n">
+        <v>865</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="n">
-        <v>10</v>
+        <v>60</v>
+      </c>
+      <c r="B99" s="0" t="n">
+        <v>2184</v>
+      </c>
+      <c r="C99" s="0" t="n">
+        <v>1497</v>
+      </c>
+      <c r="D99" s="0" t="n">
+        <v>1486</v>
+      </c>
+      <c r="E99" s="0" t="n">
+        <v>857</v>
+      </c>
+      <c r="F99" s="0" t="n">
+        <v>637</v>
+      </c>
+      <c r="G99" s="0" t="n">
+        <v>992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>